<commit_message>
added Lombok sites to excel file
</commit_message>
<xml_diff>
--- a/Indonesia/All study sites - multiple maps/site_info.xlsx
+++ b/Indonesia/All study sites - multiple maps/site_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgcar\OneDrive\Documents\github\map-figures\Indonesia\All study sites - multiple maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381E2FAD-6DD7-4AD8-9D37-4AAC37905184}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6DFF91-34CA-47B1-9E13-69293C75B719}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="6">
   <si>
     <t>lon</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Wakatobi</t>
+  </si>
+  <si>
+    <t>Lombok</t>
   </si>
 </sst>
 </file>
@@ -70,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +843,204 @@
         <v>-5.4589999999999996</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1">
+        <v>116.706</v>
+      </c>
+      <c r="C41" s="1">
+        <v>-8.3179999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>116.72499999999999</v>
+      </c>
+      <c r="C42" s="1">
+        <v>-8.3149999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1">
+        <v>116.71299999999999</v>
+      </c>
+      <c r="C43" s="1">
+        <v>-8.31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1">
+        <v>116.688</v>
+      </c>
+      <c r="C44" s="1">
+        <v>-8.2970000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1">
+        <v>116.755</v>
+      </c>
+      <c r="C45" s="1">
+        <v>-8.4120000000000008</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1">
+        <v>116.73399999999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-8.4429999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1">
+        <v>116.006</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-8.7149999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1">
+        <v>116.047</v>
+      </c>
+      <c r="C48" s="1">
+        <v>-8.7279999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1">
+        <v>116.039</v>
+      </c>
+      <c r="C49" s="1">
+        <v>-8.7170000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1">
+        <v>115.919</v>
+      </c>
+      <c r="C50" s="1">
+        <v>-8.7189999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1">
+        <v>115.89</v>
+      </c>
+      <c r="C51" s="1">
+        <v>-8.7490000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
+        <v>115.916</v>
+      </c>
+      <c r="C52" s="1">
+        <v>-8.734</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1">
+        <v>115.916</v>
+      </c>
+      <c r="C53" s="1">
+        <v>-8.3539999999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>116.038</v>
+      </c>
+      <c r="C54" s="1">
+        <v>-8.3379999999999992</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1">
+        <v>116.051</v>
+      </c>
+      <c r="C55" s="1">
+        <v>-8.3480000000000008</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
+        <v>116.07299999999999</v>
+      </c>
+      <c r="C56" s="1">
+        <v>-8.3640000000000008</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1">
+        <v>116.108</v>
+      </c>
+      <c r="C57" s="1">
+        <v>-8.3580000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="1">
+        <v>116.09699999999999</v>
+      </c>
+      <c r="C58" s="1">
+        <v>-8.3670000000000009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>